<commit_message>
Add sprint 3 beginning
</commit_message>
<xml_diff>
--- a/deliverables/Project07/Team02Report.xlsx
+++ b/deliverables/Project07/Team02Report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/justin/proj/gedcom-linter/deliverables/Project07/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03C824C2-A233-6849-A664-D39A3EF65E0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E6D5FC4-F244-2444-A6C9-F521E2957599}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7720" yWindow="20" windowWidth="33240" windowHeight="25600" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5400" yWindow="1800" windowWidth="33240" windowHeight="25600" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -3220,7 +3220,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>